<commit_message>
añadido logica para la temporada 2006
</commit_message>
<xml_diff>
--- a/Excels/main_list.xlsx
+++ b/Excels/main_list.xlsx
@@ -8,14 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zaka\Desktop\MOTOGP\Excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDF324AB-E636-4131-9B1F-F9BE5E24BE41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5355F88A-B807-4726-B7DD-3C6ADA7A50AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{B5FA4BD0-4BC3-4586-95F1-1E5EE0137B00}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{B5FA4BD0-4BC3-4586-95F1-1E5EE0137B00}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="10">
   <si>
     <t>file_name</t>
   </si>
@@ -52,6 +54,18 @@
   </si>
   <si>
     <t>C:\Users\zaka\Desktop\MOTOGP\Excels\data\2003.xlsx</t>
+  </si>
+  <si>
+    <t>C:\Users\zaka\Desktop\MOTOGP\Excels\data\2005.xlsx</t>
+  </si>
+  <si>
+    <t>2005</t>
+  </si>
+  <si>
+    <t>C:\Users\zaka\Desktop\MOTOGP\Excels\data\2006.xlsx</t>
+  </si>
+  <si>
+    <t>2006</t>
   </si>
 </sst>
 </file>
@@ -410,10 +424,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06742978-E384-4409-B461-AA567BB406DC}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -446,8 +460,82 @@
         <v>3</v>
       </c>
     </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91A9C7F2-6FF4-42EB-925A-F65480154845}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="51" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
añadido el 2002, falta logica para Akira Ryo
</commit_message>
<xml_diff>
--- a/Excels/main_list.xlsx
+++ b/Excels/main_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zaka\Desktop\MOTOGP\Excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5355F88A-B807-4726-B7DD-3C6ADA7A50AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{408A6ED4-66B5-4C75-9302-180F70F68468}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{B5FA4BD0-4BC3-4586-95F1-1E5EE0137B00}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
   <si>
     <t>file_name</t>
   </si>
@@ -66,6 +66,24 @@
   </si>
   <si>
     <t>2006</t>
+  </si>
+  <si>
+    <t>C:\Users\zaka\Desktop\MOTOGP\Excels\data\2007.xlsx</t>
+  </si>
+  <si>
+    <t>2007</t>
+  </si>
+  <si>
+    <t>C:\Users\zaka\Desktop\MOTOGP\Excels\data\2008.xlsx</t>
+  </si>
+  <si>
+    <t>2008</t>
+  </si>
+  <si>
+    <t>2002</t>
+  </si>
+  <si>
+    <t>C:\Users\zaka\Desktop\MOTOGP\Excels\data\2002.xlsx</t>
   </si>
 </sst>
 </file>
@@ -107,9 +125,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -424,10 +444,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06742978-E384-4409-B461-AA567BB406DC}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -446,48 +466,29 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>9</v>
-      </c>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="3"/>
+      <c r="B7" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91A9C7F2-6FF4-42EB-925A-F65480154845}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B5"/>
+      <selection activeCell="A2" sqref="A2:B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -535,6 +536,22 @@
         <v>9</v>
       </c>
     </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
añadida logica y datos hasta la temporada 2010, solucionados los temas de multiples nombres de equipo en una temporada desde los propios datos
</commit_message>
<xml_diff>
--- a/Excels/main_list.xlsx
+++ b/Excels/main_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zaka\Desktop\MOTOGP\Excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{408A6ED4-66B5-4C75-9302-180F70F68468}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FE130AA-FD35-462F-8A73-6972F0BEBB68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{B5FA4BD0-4BC3-4586-95F1-1E5EE0137B00}"/>
   </bookViews>
@@ -17,7 +17,6 @@
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="20">
   <si>
     <t>file_name</t>
   </si>
@@ -84,6 +83,18 @@
   </si>
   <si>
     <t>C:\Users\zaka\Desktop\MOTOGP\Excels\data\2002.xlsx</t>
+  </si>
+  <si>
+    <t>C:\Users\zaka\Desktop\MOTOGP\Excels\data\2009.xlsx</t>
+  </si>
+  <si>
+    <t>2009</t>
+  </si>
+  <si>
+    <t>C:\Users\zaka\Desktop\MOTOGP\Excels\data\2010.xlsx</t>
+  </si>
+  <si>
+    <t>2010</t>
   </si>
 </sst>
 </file>
@@ -125,11 +136,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -444,10 +453,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06742978-E384-4409-B461-AA567BB406DC}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A2" sqref="A2:B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -472,9 +481,69 @@
         <v>14</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
-      <c r="B7" s="2"/>
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>19</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -485,10 +554,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91A9C7F2-6FF4-42EB-925A-F65480154845}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B7"/>
+      <selection activeCell="A2" sqref="A2:B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -506,50 +575,74 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B7" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B8" s="1" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
añadia la logica para el 2012, junto a la logica de CRT/prototipo y la actualizacion de la localizacion de los cirtuitos
</commit_message>
<xml_diff>
--- a/Excels/main_list.xlsx
+++ b/Excels/main_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zaka\Desktop\MOTOGP\Excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FE130AA-FD35-462F-8A73-6972F0BEBB68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C53839B-8D85-4E6C-9730-1022C2765CE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{B5FA4BD0-4BC3-4586-95F1-1E5EE0137B00}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="24">
   <si>
     <t>file_name</t>
   </si>
@@ -95,6 +95,18 @@
   </si>
   <si>
     <t>2010</t>
+  </si>
+  <si>
+    <t>C:\Users\zaka\Desktop\MOTOGP\Excels\data\2011.xlsx</t>
+  </si>
+  <si>
+    <t>2011</t>
+  </si>
+  <si>
+    <t>C:\Users\zaka\Desktop\MOTOGP\Excels\data\2012.xlsx</t>
+  </si>
+  <si>
+    <t>2012</t>
   </si>
 </sst>
 </file>
@@ -453,10 +465,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06742978-E384-4409-B461-AA567BB406DC}">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B10"/>
+      <selection activeCell="A2" sqref="A2:B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -545,6 +557,22 @@
         <v>19</v>
       </c>
     </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -554,10 +582,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91A9C7F2-6FF4-42EB-925A-F65480154845}">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B10"/>
+      <selection activeCell="A2" sqref="A2:B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -645,6 +673,22 @@
         <v>19</v>
       </c>
     </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
actualizada la lógica hasta el año 2017
</commit_message>
<xml_diff>
--- a/Excels/main_list.xlsx
+++ b/Excels/main_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zaka\Desktop\MOTOGP\Excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C53839B-8D85-4E6C-9730-1022C2765CE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{388625A9-CE6F-44AB-B8F4-8DB45CCF706F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{B5FA4BD0-4BC3-4586-95F1-1E5EE0137B00}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="16200" windowHeight="9360" xr2:uid="{B5FA4BD0-4BC3-4586-95F1-1E5EE0137B00}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="34">
   <si>
     <t>file_name</t>
   </si>
@@ -107,6 +107,36 @@
   </si>
   <si>
     <t>2012</t>
+  </si>
+  <si>
+    <t>C:\Users\zaka\Desktop\MOTOGP\Excels\data\2013.xlsx</t>
+  </si>
+  <si>
+    <t>2013</t>
+  </si>
+  <si>
+    <t>C:\Users\zaka\Desktop\MOTOGP\Excels\data\2014.xlsx</t>
+  </si>
+  <si>
+    <t>2014</t>
+  </si>
+  <si>
+    <t>C:\Users\zaka\Desktop\MOTOGP\Excels\data\2015.xlsx</t>
+  </si>
+  <si>
+    <t>2015</t>
+  </si>
+  <si>
+    <t>C:\Users\zaka\Desktop\MOTOGP\Excels\data\2016.xlsx</t>
+  </si>
+  <si>
+    <t>2016</t>
+  </si>
+  <si>
+    <t>C:\Users\zaka\Desktop\MOTOGP\Excels\data\2017.xlsx</t>
+  </si>
+  <si>
+    <t>2017</t>
   </si>
 </sst>
 </file>
@@ -465,10 +495,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06742978-E384-4409-B461-AA567BB406DC}">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B12"/>
+      <selection activeCell="A2" sqref="A2:B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -573,6 +603,46 @@
         <v>23</v>
       </c>
     </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -582,10 +652,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91A9C7F2-6FF4-42EB-925A-F65480154845}">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B12"/>
+      <selection activeCell="A2" sqref="A2:B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -689,6 +759,46 @@
         <v>23</v>
       </c>
     </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
version operativa para sacar poles y FL
</commit_message>
<xml_diff>
--- a/Excels/main_list.xlsx
+++ b/Excels/main_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zaka\Desktop\MOTOGP\Excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{388625A9-CE6F-44AB-B8F4-8DB45CCF706F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{139D3D42-88D4-4621-92F0-A7F56F8B415A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="16200" windowHeight="9360" xr2:uid="{B5FA4BD0-4BC3-4586-95F1-1E5EE0137B00}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{B5FA4BD0-4BC3-4586-95F1-1E5EE0137B00}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="36">
   <si>
     <t>file_name</t>
   </si>
@@ -137,6 +137,12 @@
   </si>
   <si>
     <t>2017</t>
+  </si>
+  <si>
+    <t>C:\Users\zaka\Desktop\MOTOGP\Excels\data\2018.xlsx</t>
+  </si>
+  <si>
+    <t>2018</t>
   </si>
 </sst>
 </file>
@@ -495,10 +501,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06742978-E384-4409-B461-AA567BB406DC}">
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B17"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -517,130 +523,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>22</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>24</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>26</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>28</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>30</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>32</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Añadida la logica hasta 2020
</commit_message>
<xml_diff>
--- a/Excels/main_list.xlsx
+++ b/Excels/main_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zaka\Desktop\MOTOGP\Excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{139D3D42-88D4-4621-92F0-A7F56F8B415A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5C670A0-208A-4F28-94FF-E4302821B001}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{B5FA4BD0-4BC3-4586-95F1-1E5EE0137B00}"/>
+    <workbookView xWindow="-8055" yWindow="4770" windowWidth="16200" windowHeight="9360" xr2:uid="{B5FA4BD0-4BC3-4586-95F1-1E5EE0137B00}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="40">
   <si>
     <t>file_name</t>
   </si>
@@ -143,6 +143,18 @@
   </si>
   <si>
     <t>2018</t>
+  </si>
+  <si>
+    <t>C:\Users\zaka\Desktop\MOTOGP\Excels\data\2019.xlsx</t>
+  </si>
+  <si>
+    <t>2019</t>
+  </si>
+  <si>
+    <t>2020</t>
+  </si>
+  <si>
+    <t>C:\Users\zaka\Desktop\MOTOGP\Excels\data\2020.xlsx</t>
   </si>
 </sst>
 </file>
@@ -501,10 +513,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06742978-E384-4409-B461-AA567BB406DC}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -523,10 +535,154 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B18" s="1" t="s">
         <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>39</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -538,10 +694,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91A9C7F2-6FF4-42EB-925A-F65480154845}">
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B17"/>
+      <selection activeCell="A2" sqref="A2:B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -685,6 +841,30 @@
         <v>33</v>
       </c>
     </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>39</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
añadida logica hasta 2022, queda 2023: El Regex de la muerte
</commit_message>
<xml_diff>
--- a/Excels/main_list.xlsx
+++ b/Excels/main_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zaka\Desktop\MOTOGP\Excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5C670A0-208A-4F28-94FF-E4302821B001}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75EAF95B-446D-42A7-9919-D3CB0DB60E16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-8055" yWindow="4770" windowWidth="16200" windowHeight="9360" xr2:uid="{B5FA4BD0-4BC3-4586-95F1-1E5EE0137B00}"/>
+    <workbookView xWindow="2595" yWindow="2595" windowWidth="16200" windowHeight="9360" xr2:uid="{B5FA4BD0-4BC3-4586-95F1-1E5EE0137B00}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="44">
   <si>
     <t>file_name</t>
   </si>
@@ -155,6 +155,18 @@
   </si>
   <si>
     <t>C:\Users\zaka\Desktop\MOTOGP\Excels\data\2020.xlsx</t>
+  </si>
+  <si>
+    <t>C:\Users\zaka\Desktop\MOTOGP\Excels\data\2021.xlsx</t>
+  </si>
+  <si>
+    <t>2021</t>
+  </si>
+  <si>
+    <t>C:\Users\zaka\Desktop\MOTOGP\Excels\data\2022.xlsx</t>
+  </si>
+  <si>
+    <t>2022</t>
   </si>
 </sst>
 </file>
@@ -513,10 +525,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06742978-E384-4409-B461-AA567BB406DC}">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="A2" sqref="A2:B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -685,6 +697,22 @@
         <v>38</v>
       </c>
     </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -694,10 +722,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91A9C7F2-6FF4-42EB-925A-F65480154845}">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B20"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -865,6 +893,22 @@
         <v>38</v>
       </c>
     </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
cambiados los datos a mano del 2023, hay que sacarlos bien usando la api
</commit_message>
<xml_diff>
--- a/Excels/main_list.xlsx
+++ b/Excels/main_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zaka\Desktop\MOTOGP\Excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75EAF95B-446D-42A7-9919-D3CB0DB60E16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69896BCD-08D0-4E04-B701-7A97752740BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2595" yWindow="2595" windowWidth="16200" windowHeight="9360" xr2:uid="{B5FA4BD0-4BC3-4586-95F1-1E5EE0137B00}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="18075" windowHeight="12255" xr2:uid="{B5FA4BD0-4BC3-4586-95F1-1E5EE0137B00}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="46">
   <si>
     <t>file_name</t>
   </si>
@@ -167,6 +167,12 @@
   </si>
   <si>
     <t>2022</t>
+  </si>
+  <si>
+    <t>C:\Users\zaka\Desktop\MOTOGP\Excels\data\2023.xlsx</t>
+  </si>
+  <si>
+    <t>2023</t>
   </si>
 </sst>
 </file>
@@ -525,10 +531,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06742978-E384-4409-B461-AA567BB406DC}">
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B22"/>
+      <selection activeCell="A2" sqref="A2:B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -713,6 +719,14 @@
         <v>43</v>
       </c>
     </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -722,10 +736,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91A9C7F2-6FF4-42EB-925A-F65480154845}">
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:B23"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -909,6 +923,14 @@
         <v>43</v>
       </c>
     </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
añadidos datos de 125 y 250 a 2002.xlsx y sus inputs. Funciona OK
</commit_message>
<xml_diff>
--- a/Excels/main_list.xlsx
+++ b/Excels/main_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zaka\Desktop\MOTOGP\Excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69896BCD-08D0-4E04-B701-7A97752740BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19E603E0-AC22-45E3-A759-AAA8BA878394}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="18075" windowHeight="12255" xr2:uid="{B5FA4BD0-4BC3-4586-95F1-1E5EE0137B00}"/>
+    <workbookView xWindow="2730" yWindow="2730" windowWidth="18075" windowHeight="12255" xr2:uid="{B5FA4BD0-4BC3-4586-95F1-1E5EE0137B00}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="46">
   <si>
     <t>file_name</t>
   </si>
@@ -531,10 +531,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06742978-E384-4409-B461-AA567BB406DC}">
-  <dimension ref="A1:B23"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B23"/>
+      <selection activeCell="A3" sqref="A3:B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -557,174 +557,6 @@
       </c>
       <c r="B2" s="1" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>22</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>24</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>26</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>28</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>30</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>32</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>34</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>36</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>39</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>40</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>42</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>44</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
añadidos 125 y 250 hasta 2004
</commit_message>
<xml_diff>
--- a/Excels/main_list.xlsx
+++ b/Excels/main_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zaka\Desktop\MOTOGP\Excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15947552-B7C9-4C1D-A2A4-F7A2F82D99E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{959C009D-6F7D-45EC-BCB6-741D1C5D3E05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3075" yWindow="3075" windowWidth="18075" windowHeight="12255" xr2:uid="{B5FA4BD0-4BC3-4586-95F1-1E5EE0137B00}"/>
+    <workbookView xWindow="3030" yWindow="3030" windowWidth="18075" windowHeight="12255" xr2:uid="{B5FA4BD0-4BC3-4586-95F1-1E5EE0137B00}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
añadidos 125 y 250 hasta 2005
</commit_message>
<xml_diff>
--- a/Excels/main_list.xlsx
+++ b/Excels/main_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zaka\Desktop\MOTOGP\Excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{959C009D-6F7D-45EC-BCB6-741D1C5D3E05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E973009-508F-4774-B279-F034902A3AB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3030" yWindow="3030" windowWidth="18075" windowHeight="12255" xr2:uid="{B5FA4BD0-4BC3-4586-95F1-1E5EE0137B00}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="18075" windowHeight="12255" xr2:uid="{B5FA4BD0-4BC3-4586-95F1-1E5EE0137B00}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
añadido 125 y 250 hasta 2006
</commit_message>
<xml_diff>
--- a/Excels/main_list.xlsx
+++ b/Excels/main_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zaka\Desktop\MOTOGP\Excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E973009-508F-4774-B279-F034902A3AB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C702ACB-A14A-4B2A-89F8-6B45C705A2AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="18075" windowHeight="12255" xr2:uid="{B5FA4BD0-4BC3-4586-95F1-1E5EE0137B00}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="18075" windowHeight="12255" xr2:uid="{B5FA4BD0-4BC3-4586-95F1-1E5EE0137B00}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
añadidos 125 y 250 a 2008
</commit_message>
<xml_diff>
--- a/Excels/main_list.xlsx
+++ b/Excels/main_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zaka\Desktop\MOTOGP\Excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD01E4C4-A627-46AB-8477-DD85E98D0192}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9CEADF3-7F5F-4F75-A059-470BF26C6083}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="18075" windowHeight="12255" xr2:uid="{B5FA4BD0-4BC3-4586-95F1-1E5EE0137B00}"/>
+    <workbookView xWindow="1515" yWindow="1515" windowWidth="18075" windowHeight="12255" xr2:uid="{B5FA4BD0-4BC3-4586-95F1-1E5EE0137B00}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="46">
   <si>
     <t>file_name</t>
   </si>
@@ -531,10 +531,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06742978-E384-4409-B461-AA567BB406DC}">
-  <dimension ref="A1:B23"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B23"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -553,178 +553,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="1" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>22</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>24</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>26</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>28</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>30</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>32</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>34</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>36</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>39</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>40</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>42</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>44</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
añadidos 125 y 250 a 2009
</commit_message>
<xml_diff>
--- a/Excels/main_list.xlsx
+++ b/Excels/main_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zaka\Desktop\MOTOGP\Excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9CEADF3-7F5F-4F75-A059-470BF26C6083}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABD86020-780B-46E8-ABEB-8019F9D0B4DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1515" yWindow="1515" windowWidth="18075" windowHeight="12255" xr2:uid="{B5FA4BD0-4BC3-4586-95F1-1E5EE0137B00}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="46">
   <si>
     <t>file_name</t>
   </si>
@@ -531,10 +531,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06742978-E384-4409-B461-AA567BB406DC}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A2" sqref="A2:B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -553,10 +553,178 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B8" s="1" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>39</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
añadidos 125 y 250 a 2010
</commit_message>
<xml_diff>
--- a/Excels/main_list.xlsx
+++ b/Excels/main_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zaka\Desktop\MOTOGP\Excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABD86020-780B-46E8-ABEB-8019F9D0B4DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{069083A0-1DAF-4554-8285-D7643D679736}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1515" yWindow="1515" windowWidth="18075" windowHeight="12255" xr2:uid="{B5FA4BD0-4BC3-4586-95F1-1E5EE0137B00}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="18075" windowHeight="12255" xr2:uid="{B5FA4BD0-4BC3-4586-95F1-1E5EE0137B00}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
Se salta 2011 por los problemas en recuperar el rider_id_fk de Raffaele de Rosa. Añadidos moto2 y moto3 a 2011 y 2012
</commit_message>
<xml_diff>
--- a/Excels/main_list.xlsx
+++ b/Excels/main_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zaka\Desktop\MOTOGP\Excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{069083A0-1DAF-4554-8285-D7643D679736}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEF15AF1-F722-4398-A172-423490EFFBB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="18075" windowHeight="12255" xr2:uid="{B5FA4BD0-4BC3-4586-95F1-1E5EE0137B00}"/>
+    <workbookView xWindow="570" yWindow="2295" windowWidth="18075" windowHeight="12255" xr2:uid="{B5FA4BD0-4BC3-4586-95F1-1E5EE0137B00}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="46">
   <si>
     <t>file_name</t>
   </si>
@@ -531,10 +531,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06742978-E384-4409-B461-AA567BB406DC}">
-  <dimension ref="A1:B23"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B23"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -553,178 +553,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>22</v>
-      </c>
-      <c r="B12" s="1" t="s">
         <v>23</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>24</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>26</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>28</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>30</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>32</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>34</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>36</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>39</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>40</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>42</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>44</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
añadido moto2 y moto3 a 2013
</commit_message>
<xml_diff>
--- a/Excels/main_list.xlsx
+++ b/Excels/main_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zaka\Desktop\MOTOGP\Excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEF15AF1-F722-4398-A172-423490EFFBB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{899F00B0-C7CC-4DE7-9B85-9C33ABBA47E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="570" yWindow="2295" windowWidth="18075" windowHeight="12255" xr2:uid="{B5FA4BD0-4BC3-4586-95F1-1E5EE0137B00}"/>
+    <workbookView xWindow="3795" yWindow="3000" windowWidth="18075" windowHeight="12255" xr2:uid="{B5FA4BD0-4BC3-4586-95F1-1E5EE0137B00}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -534,7 +534,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -553,10 +553,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
añadidos moto2 y moto3 a 2014
</commit_message>
<xml_diff>
--- a/Excels/main_list.xlsx
+++ b/Excels/main_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zaka\Desktop\MOTOGP\Excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{899F00B0-C7CC-4DE7-9B85-9C33ABBA47E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F37632C5-3F8A-461D-91F5-6F6D7786CBE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3795" yWindow="3000" windowWidth="18075" windowHeight="12255" xr2:uid="{B5FA4BD0-4BC3-4586-95F1-1E5EE0137B00}"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="18075" windowHeight="12255" xr2:uid="{B5FA4BD0-4BC3-4586-95F1-1E5EE0137B00}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -534,7 +534,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -553,10 +553,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
añadido moto2 y moto3 a 2015
</commit_message>
<xml_diff>
--- a/Excels/main_list.xlsx
+++ b/Excels/main_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zaka\Desktop\MOTOGP\Excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F37632C5-3F8A-461D-91F5-6F6D7786CBE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD571A39-0B76-4A4E-BF9E-CB3A1E0F9B15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3120" windowWidth="18075" windowHeight="12255" xr2:uid="{B5FA4BD0-4BC3-4586-95F1-1E5EE0137B00}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="18075" windowHeight="12255" xr2:uid="{B5FA4BD0-4BC3-4586-95F1-1E5EE0137B00}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -534,7 +534,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -556,7 +556,7 @@
         <v>26</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
añadido moto2 y moto3 a 2016
</commit_message>
<xml_diff>
--- a/Excels/main_list.xlsx
+++ b/Excels/main_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zaka\Desktop\MOTOGP\Excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD571A39-0B76-4A4E-BF9E-CB3A1E0F9B15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{456A55F8-2673-4A27-9481-0FFB79700DDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="18075" windowHeight="12255" xr2:uid="{B5FA4BD0-4BC3-4586-95F1-1E5EE0137B00}"/>
+    <workbookView xWindow="1905" yWindow="1905" windowWidth="18075" windowHeight="12255" xr2:uid="{B5FA4BD0-4BC3-4586-95F1-1E5EE0137B00}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -556,7 +556,7 @@
         <v>26</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
añadidos moto2 y moto3 a 2017
</commit_message>
<xml_diff>
--- a/Excels/main_list.xlsx
+++ b/Excels/main_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zaka\Desktop\MOTOGP\Excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{456A55F8-2673-4A27-9481-0FFB79700DDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75D48070-E658-4602-BF25-DB9B86D2C488}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1905" yWindow="1905" windowWidth="18075" windowHeight="12255" xr2:uid="{B5FA4BD0-4BC3-4586-95F1-1E5EE0137B00}"/>
+    <workbookView xWindow="2250" yWindow="2250" windowWidth="18075" windowHeight="12255" xr2:uid="{B5FA4BD0-4BC3-4586-95F1-1E5EE0137B00}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -556,7 +556,7 @@
         <v>26</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
añadidos moto2 y moto3 a 2018
</commit_message>
<xml_diff>
--- a/Excels/main_list.xlsx
+++ b/Excels/main_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zaka\Desktop\MOTOGP\Excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75D48070-E658-4602-BF25-DB9B86D2C488}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A251EEE-3281-4770-ADD8-5C7652A92AC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2250" yWindow="2250" windowWidth="18075" windowHeight="12255" xr2:uid="{B5FA4BD0-4BC3-4586-95F1-1E5EE0137B00}"/>
+    <workbookView xWindow="2595" yWindow="2595" windowWidth="18075" windowHeight="12255" xr2:uid="{B5FA4BD0-4BC3-4586-95F1-1E5EE0137B00}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -556,7 +556,7 @@
         <v>26</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
añadidos moto2, moto3, y motoE a 2019 y 2020
</commit_message>
<xml_diff>
--- a/Excels/main_list.xlsx
+++ b/Excels/main_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zaka\Desktop\MOTOGP\Excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A251EEE-3281-4770-ADD8-5C7652A92AC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FD8E1FA-10BD-491D-987F-A4D3BC16257B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2595" yWindow="2595" windowWidth="18075" windowHeight="12255" xr2:uid="{B5FA4BD0-4BC3-4586-95F1-1E5EE0137B00}"/>
+    <workbookView xWindow="3150" yWindow="3150" windowWidth="18075" windowHeight="12255" xr2:uid="{B5FA4BD0-4BC3-4586-95F1-1E5EE0137B00}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -553,10 +553,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -571,7 +571,7 @@
   <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B23"/>
+      <selection activeCell="A11" sqref="A11:B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
añadidos moto2, moto3 y motoe a 2021
</commit_message>
<xml_diff>
--- a/Excels/main_list.xlsx
+++ b/Excels/main_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zaka\Desktop\MOTOGP\Excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FD8E1FA-10BD-491D-987F-A4D3BC16257B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E33BC76E-9A42-4DFD-A070-4F4AC3C7956A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3150" yWindow="3150" windowWidth="18075" windowHeight="12255" xr2:uid="{B5FA4BD0-4BC3-4586-95F1-1E5EE0137B00}"/>
+    <workbookView xWindow="1515" yWindow="1515" windowWidth="18075" windowHeight="12255" xr2:uid="{B5FA4BD0-4BC3-4586-95F1-1E5EE0137B00}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -556,7 +556,7 @@
         <v>20</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
añadidos moto2, moto3 y motoe a 2022
</commit_message>
<xml_diff>
--- a/Excels/main_list.xlsx
+++ b/Excels/main_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zaka\Desktop\MOTOGP\Excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E33BC76E-9A42-4DFD-A070-4F4AC3C7956A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13A17BDF-0233-4B18-8E85-29B29C8590D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1515" yWindow="1515" windowWidth="18075" windowHeight="12255" xr2:uid="{B5FA4BD0-4BC3-4586-95F1-1E5EE0137B00}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="18075" windowHeight="12255" xr2:uid="{B5FA4BD0-4BC3-4586-95F1-1E5EE0137B00}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -556,7 +556,7 @@
         <v>20</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
añadido moto2, moto3 y motoe al 2023
</commit_message>
<xml_diff>
--- a/Excels/main_list.xlsx
+++ b/Excels/main_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zaka\Desktop\MOTOGP\Excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13A17BDF-0233-4B18-8E85-29B29C8590D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0FA8399-A651-46EC-92E7-DB87C134653E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="18075" windowHeight="12255" xr2:uid="{B5FA4BD0-4BC3-4586-95F1-1E5EE0137B00}"/>
+    <workbookView xWindow="2685" yWindow="2685" windowWidth="18075" windowHeight="12255" xr2:uid="{B5FA4BD0-4BC3-4586-95F1-1E5EE0137B00}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -556,7 +556,7 @@
         <v>20</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
añadidos mas datos biograficos
</commit_message>
<xml_diff>
--- a/Excels/main_list.xlsx
+++ b/Excels/main_list.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zaka\Desktop\MOTOGP\Excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F8013A6-79CD-4DCF-8E3B-E14FA01BB802}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1C4DB73-07BF-4000-A7AE-4AEA4D4537B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3030" yWindow="3030" windowWidth="18075" windowHeight="12255" xr2:uid="{B5FA4BD0-4BC3-4586-95F1-1E5EE0137B00}"/>
+    <workbookView xWindow="8325" yWindow="1710" windowWidth="28800" windowHeight="11385" xr2:uid="{B5FA4BD0-4BC3-4586-95F1-1E5EE0137B00}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -534,7 +534,7 @@
   <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B23"/>
+      <selection activeCell="A22" sqref="A2:XFD22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>